<commit_message>
Added initial debug database state
</commit_message>
<xml_diff>
--- a/doc/assessment_display_permissions.xlsx
+++ b/doc/assessment_display_permissions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="64">
   <si>
     <t xml:space="preserve">Pour 1 exos sur tous les assessments</t>
   </si>
@@ -73,16 +73,37 @@
     <t xml:space="preserve">R-A</t>
   </si>
   <si>
+    <t xml:space="preserve">USER_1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USER_123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USER_234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USER_134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USER_124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USER_23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USER_24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USER_34</t>
+  </si>
+  <si>
     <t xml:space="preserve">USER_12</t>
   </si>
   <si>
     <t xml:space="preserve">USER_13</t>
   </si>
   <si>
-    <t xml:space="preserve">USER_23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USER_123</t>
+    <t xml:space="preserve">USER_14</t>
   </si>
   <si>
     <t xml:space="preserve">USER_1</t>
@@ -94,28 +115,31 @@
     <t xml:space="preserve">USER_3</t>
   </si>
   <si>
-    <t xml:space="preserve">Assess T3 ALL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assess P3 ALL</t>
+    <t xml:space="preserve">USER_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assess T4 ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asses C3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asses F3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assess P4 ALL</t>
   </si>
   <si>
     <t xml:space="preserve">T : start&lt;end&lt;training&lt;current</t>
   </si>
   <si>
-    <t xml:space="preserve">Assess T2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Asses P2</t>
   </si>
   <si>
     <t xml:space="preserve">Asses C2</t>
   </si>
   <si>
-    <t xml:space="preserve">Assess F2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assess C3 ALL</t>
+    <t xml:space="preserve">Assess C4 ALL</t>
   </si>
   <si>
     <t xml:space="preserve">P : start&lt;end&lt;current&lt;training</t>
@@ -127,13 +151,7 @@
     <t xml:space="preserve">Asses P1</t>
   </si>
   <si>
-    <t xml:space="preserve">Asses C1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assess F1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assess F3 ALL</t>
+    <t xml:space="preserve">Assess F4 ALL</t>
   </si>
   <si>
     <t xml:space="preserve">E : start&lt;current&lt;end&lt;training</t>
@@ -440,11 +458,11 @@
   </sheetPr>
   <dimension ref="A2:AE1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U16" activeCellId="0" sqref="U16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S15" activeCellId="0" sqref="S15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="18.61"/>
@@ -464,7 +482,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="4.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="3.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="3.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="5.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="5.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="5.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="7.68"/>
   </cols>
@@ -548,6 +566,21 @@
       <c r="K5" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="O5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
@@ -917,6 +950,9 @@
       </c>
       <c r="R14" s="5" t="n">
         <v>15</v>
+      </c>
+      <c r="S14" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -944,6 +980,18 @@
       <c r="L15" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="S15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T15" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="U15" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="V15" s="0" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
@@ -969,6 +1017,15 @@
       </c>
       <c r="L16" s="0" t="n">
         <v>12</v>
+      </c>
+      <c r="S16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="T16" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="U16" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -996,6 +1053,15 @@
       <c r="L17" s="0" t="n">
         <v>13</v>
       </c>
+      <c r="S17" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="T17" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="U17" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="n">
@@ -1023,16 +1089,16 @@
         <v>14</v>
       </c>
       <c r="S18" s="0" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="T18" s="0" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="U18" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="V18" s="0" t="s">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="W18" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1060,15 +1126,6 @@
       <c r="L19" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="S19" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="T19" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="U19" s="0" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -1093,101 +1150,118 @@
         <v>10</v>
       </c>
       <c r="W20" s="0" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="U21" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="V21" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="W21" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="S22" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="S22" s="5"/>
       <c r="T22" s="5" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="U22" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="V22" s="0" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="W22" s="0" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="S23" s="5" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="T23" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="U23" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="V23" s="0" t="s">
-        <v>36</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="U23" s="5"/>
       <c r="W23" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
+      </c>
+      <c r="Y24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB24" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC24" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD24" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE24" s="0" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="S25" s="6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="T25" s="6" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="U25" s="6" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="V25" s="6" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="W25" s="6" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="X25" s="7" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="Y25" s="6" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="Z25" s="6" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="AA25" s="6" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="AB25" s="6" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="AC25" s="6" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="AD25" s="6" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="AE25" s="6" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1214,7 +1288,7 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="T27" s="8" t="s">
         <v>10</v>
@@ -1239,7 +1313,7 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="U28" s="8" t="s">
         <v>10</v>
@@ -1264,7 +1338,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="V29" s="8" t="s">
         <v>10</v>
@@ -1289,7 +1363,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="S30" s="8" t="s">
         <v>10</v>
@@ -1317,7 +1391,7 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="T31" s="8" t="s">
         <v>10</v>

</xml_diff>